<commit_message>
Se termina tarjeta de credito
</commit_message>
<xml_diff>
--- a/docs/CasosPrueba - Validación/CP - Tarjeta Crédito.xlsx
+++ b/docs/CasosPrueba - Validación/CP - Tarjeta Crédito.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adri_\source\repos\TDD-ACB-JGA\docs\CasosPrueba - Validación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C4E981-B56E-4DB5-88BD-7B52B7F70023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9A521D-40CE-4F2E-8240-112CAFE17689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
+    <workbookView xWindow="4365" yWindow="1350" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
   </bookViews>
   <sheets>
     <sheet name="CP-VAL-TC-001" sheetId="1" r:id="rId1"/>
@@ -290,15 +290,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -318,15 +327,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -764,10 +764,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -779,10 +779,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -792,10 +792,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -807,13 +807,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
@@ -839,71 +839,71 @@
       <c r="F8" s="23"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -915,10 +915,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7">
         <v>0</v>
       </c>
@@ -930,8 +930,8 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -939,8 +939,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -957,65 +957,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1026,13 +1026,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C22:F22"/>
     <mergeCell ref="B4:C4"/>
@@ -1049,6 +1042,13 @@
     <mergeCell ref="C20:F20"/>
     <mergeCell ref="B6:F8"/>
     <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -1083,10 +1083,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1098,10 +1098,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1111,10 +1111,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1126,13 +1126,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -1158,73 +1158,73 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1236,10 +1236,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7">
         <v>0</v>
       </c>
@@ -1251,8 +1251,8 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -1260,8 +1260,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1278,65 +1278,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1347,12 +1347,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F25"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -1365,11 +1364,12 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -1391,7 +1391,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:F11"/>
+      <selection activeCell="B6" sqref="B6:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,10 +1404,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="10"/>
       <c r="D2" s="4" t="s">
         <v>20</v>
       </c>
@@ -1419,10 +1419,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1432,10 +1432,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1447,13 +1447,13 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
@@ -1479,73 +1479,73 @@
       <c r="F8" s="24"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1557,10 +1557,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7">
         <v>1</v>
       </c>
@@ -1572,8 +1572,8 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -1581,8 +1581,8 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
     </row>
@@ -1599,65 +1599,65 @@
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>2</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="12" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="13"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1668,12 +1668,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="D24:F25"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -1686,11 +1685,12 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="D24:F25"/>
-    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D26">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>